<commit_message>
Working on rubric more
</commit_message>
<xml_diff>
--- a/Rubric/GAM_Project_Rubric_Final.xlsx
+++ b/Rubric/GAM_Project_Rubric_Final.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="903">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3405,30 +3405,6 @@
   </si>
   <si>
     <t>I spend most of my time developing the game on a Surface Pro 3, which has an Intel HD5000 GPU. The game runs flawlessly on this machine. 60FPS most of the time.</t>
-  </si>
-  <si>
-    <t>%APPDATA%\DigiPen\... Is fine, I assume?</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">git clean </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and done</t>
-    </r>
   </si>
   <si>
     <r>
@@ -5225,19 +5201,31 @@
     <xf numFmtId="0" fontId="28" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5249,22 +5237,43 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="26" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5294,76 +5303,82 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5384,45 +5399,6 @@
     <xf numFmtId="9" fontId="4" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5432,6 +5408,33 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5439,42 +5442,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5513,32 +5480,41 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -24065,54 +24041,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14" customHeight="1" thickBot="1">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="137"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="148"/>
       <c r="E1" s="16"/>
-      <c r="F1" s="135" t="s">
+      <c r="F1" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="137"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="148"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="32"/>
     </row>
     <row r="2" spans="1:13" ht="14" customHeight="1">
-      <c r="A2" s="138" t="s">
-        <v>897</v>
-      </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
-      <c r="D2" s="140"/>
+      <c r="A2" s="149" t="s">
+        <v>895</v>
+      </c>
+      <c r="B2" s="150"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="151"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="138" t="s">
-        <v>898</v>
-      </c>
-      <c r="G2" s="139"/>
-      <c r="H2" s="139"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="140"/>
+      <c r="F2" s="149" t="s">
+        <v>896</v>
+      </c>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="151"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:13" ht="14" customHeight="1" thickBot="1">
-      <c r="A3" s="141"/>
-      <c r="B3" s="142"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143"/>
+      <c r="A3" s="152"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="143"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="154"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="32"/>
@@ -24133,41 +24109,41 @@
       <c r="M4" s="32"/>
     </row>
     <row r="5" spans="1:13" ht="14" customHeight="1" thickBot="1">
-      <c r="A5" s="135" t="s">
+      <c r="A5" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="137"/>
+      <c r="B5" s="147"/>
+      <c r="C5" s="147"/>
+      <c r="D5" s="148"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="135" t="s">
+      <c r="F5" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="137"/>
+      <c r="G5" s="147"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="148"/>
       <c r="K5" s="6"/>
       <c r="L5" s="27"/>
       <c r="M5" s="32"/>
     </row>
     <row r="6" spans="1:13" ht="14" customHeight="1" thickBot="1">
-      <c r="A6" s="147" t="s">
+      <c r="A6" s="143" t="s">
+        <v>897</v>
+      </c>
+      <c r="B6" s="144"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="143" t="s">
         <v>899</v>
       </c>
-      <c r="B6" s="148"/>
-      <c r="C6" s="148"/>
-      <c r="D6" s="149"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="147" t="s">
-        <v>901</v>
-      </c>
-      <c r="G6" s="148"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="149"/>
+      <c r="G6" s="144"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="144"/>
+      <c r="J6" s="145"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="144" t="s">
+      <c r="L6" s="140" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="32"/>
@@ -24178,49 +24154,49 @@
       <c r="C7" s="5"/>
       <c r="D7" s="34"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="147" t="s">
-        <v>902</v>
-      </c>
-      <c r="G7" s="148"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="149"/>
+      <c r="F7" s="143" t="s">
+        <v>900</v>
+      </c>
+      <c r="G7" s="144"/>
+      <c r="H7" s="144"/>
+      <c r="I7" s="144"/>
+      <c r="J7" s="145"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="145"/>
+      <c r="L7" s="141"/>
       <c r="M7" s="32"/>
     </row>
     <row r="8" spans="1:13" ht="14" customHeight="1" thickBot="1">
-      <c r="A8" s="135" t="s">
+      <c r="A8" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="137"/>
+      <c r="B8" s="147"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="148"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="148"/>
-      <c r="H8" s="148"/>
-      <c r="I8" s="148"/>
-      <c r="J8" s="149"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="144"/>
+      <c r="H8" s="144"/>
+      <c r="I8" s="144"/>
+      <c r="J8" s="145"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="145"/>
+      <c r="L8" s="141"/>
       <c r="M8" s="32"/>
     </row>
     <row r="9" spans="1:13" ht="14" customHeight="1" thickBot="1">
-      <c r="A9" s="147" t="s">
-        <v>900</v>
-      </c>
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="149"/>
+      <c r="A9" s="143" t="s">
+        <v>898</v>
+      </c>
+      <c r="B9" s="144"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="145"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="147"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="149"/>
+      <c r="F9" s="143"/>
+      <c r="G9" s="144"/>
+      <c r="H9" s="144"/>
+      <c r="I9" s="144"/>
+      <c r="J9" s="145"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="146"/>
+      <c r="L9" s="142"/>
       <c r="M9" s="32"/>
     </row>
     <row r="10" spans="1:13" ht="14" customHeight="1" thickBot="1">
@@ -24239,18 +24215,18 @@
       <c r="M10" s="32"/>
     </row>
     <row r="11" spans="1:13" ht="14" customHeight="1" thickBot="1">
-      <c r="A11" s="135" t="s">
+      <c r="A11" s="146" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="136"/>
-      <c r="C11" s="136"/>
-      <c r="D11" s="137"/>
+      <c r="B11" s="147"/>
+      <c r="C11" s="147"/>
+      <c r="D11" s="148"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="135" t="s">
+      <c r="F11" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="136"/>
-      <c r="H11" s="137"/>
+      <c r="G11" s="147"/>
+      <c r="H11" s="148"/>
       <c r="I11" s="2" t="s">
         <v>7</v>
       </c>
@@ -24290,7 +24266,7 @@
         <v>-0.08</v>
       </c>
       <c r="K12" s="6"/>
-      <c r="L12" s="144" t="s">
+      <c r="L12" s="140" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="32"/>
@@ -24321,7 +24297,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="44"/>
-      <c r="L13" s="145"/>
+      <c r="L13" s="141"/>
       <c r="M13" s="45"/>
     </row>
     <row r="14" spans="1:13" ht="14" customHeight="1" thickBot="1">
@@ -24349,7 +24325,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="12"/>
-      <c r="L14" s="146"/>
+      <c r="L14" s="142"/>
       <c r="M14" s="49"/>
     </row>
     <row r="15" spans="1:13" ht="14" customHeight="1" thickBot="1">
@@ -24405,11 +24381,11 @@
       <c r="C17" s="42"/>
       <c r="D17" s="43"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="135" t="s">
+      <c r="F17" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="136"/>
-      <c r="H17" s="137"/>
+      <c r="G17" s="147"/>
+      <c r="H17" s="148"/>
       <c r="I17" s="2"/>
       <c r="J17" s="35">
         <v>0.75</v>
@@ -24427,17 +24403,17 @@
       <c r="F18" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="123" t="s">
+      <c r="G18" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="124"/>
-      <c r="I18" s="125"/>
+      <c r="H18" s="158"/>
+      <c r="I18" s="159"/>
       <c r="J18" s="40">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>0</v>
       </c>
       <c r="K18" s="51"/>
-      <c r="L18" s="144" t="s">
+      <c r="L18" s="140" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="32"/>
@@ -24451,17 +24427,17 @@
       <c r="F19" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="126" t="s">
+      <c r="G19" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="127"/>
-      <c r="I19" s="128"/>
+      <c r="H19" s="131"/>
+      <c r="I19" s="132"/>
       <c r="J19" s="48">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(J11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(J11=0.15,-0.02,-0.3),IF(J11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="6"/>
-      <c r="L19" s="146"/>
+      <c r="L19" s="142"/>
       <c r="M19" s="32"/>
     </row>
     <row r="20" spans="1:13" ht="14" customHeight="1" thickBot="1">
@@ -24505,23 +24481,23 @@
       <c r="C22" s="42"/>
       <c r="D22" s="43"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="131" t="s">
+      <c r="F22" s="162" t="s">
         <v>846</v>
       </c>
-      <c r="G22" s="129">
+      <c r="G22" s="160">
         <f>'Project Grade'!$G$3</f>
         <v>0.79</v>
       </c>
-      <c r="H22" s="122"/>
+      <c r="H22" s="156"/>
       <c r="I22" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="J22" s="133">
+      <c r="J22" s="164">
         <f>J20+J15</f>
         <v>0.77</v>
       </c>
       <c r="K22" s="6"/>
-      <c r="L22" s="150" t="s">
+      <c r="L22" s="121" t="s">
         <v>25</v>
       </c>
       <c r="M22" s="32"/>
@@ -24532,15 +24508,15 @@
       <c r="C23" s="42"/>
       <c r="D23" s="43"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="132"/>
-      <c r="G23" s="130"/>
-      <c r="H23" s="122"/>
+      <c r="F23" s="163"/>
+      <c r="G23" s="161"/>
+      <c r="H23" s="156"/>
       <c r="I23" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="134"/>
+      <c r="J23" s="165"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="151"/>
+      <c r="L23" s="122"/>
       <c r="M23" s="32"/>
     </row>
     <row r="24" spans="1:13" ht="14" customHeight="1" thickBot="1">
@@ -24564,13 +24540,13 @@
       <c r="C25" s="42"/>
       <c r="D25" s="43"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="160" t="s">
+      <c r="F25" s="134" t="s">
         <v>738</v>
       </c>
-      <c r="G25" s="161"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="161"/>
-      <c r="J25" s="162"/>
+      <c r="G25" s="135"/>
+      <c r="H25" s="135"/>
+      <c r="I25" s="135"/>
+      <c r="J25" s="136"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="32"/>
@@ -24581,11 +24557,11 @@
       <c r="C26" s="42"/>
       <c r="D26" s="43"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="163"/>
-      <c r="G26" s="164"/>
-      <c r="H26" s="164"/>
-      <c r="I26" s="164"/>
-      <c r="J26" s="165"/>
+      <c r="F26" s="137"/>
+      <c r="G26" s="138"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="138"/>
+      <c r="J26" s="139"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="32"/>
@@ -24611,13 +24587,13 @@
       <c r="C28" s="42"/>
       <c r="D28" s="43"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="159" t="s">
+      <c r="F28" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="G28" s="159"/>
-      <c r="H28" s="159"/>
-      <c r="I28" s="159"/>
-      <c r="J28" s="159"/>
+      <c r="G28" s="133"/>
+      <c r="H28" s="133"/>
+      <c r="I28" s="133"/>
+      <c r="J28" s="133"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="32"/>
@@ -24628,13 +24604,13 @@
       <c r="C29" s="42"/>
       <c r="D29" s="43"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="156" t="s">
+      <c r="F29" s="127" t="s">
         <v>737</v>
       </c>
-      <c r="G29" s="157"/>
-      <c r="H29" s="157"/>
-      <c r="I29" s="157"/>
-      <c r="J29" s="158"/>
+      <c r="G29" s="128"/>
+      <c r="H29" s="128"/>
+      <c r="I29" s="128"/>
+      <c r="J29" s="129"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="32"/>
@@ -24645,28 +24621,28 @@
       <c r="C30" s="42"/>
       <c r="D30" s="43"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="156"/>
-      <c r="G30" s="157"/>
-      <c r="H30" s="157"/>
-      <c r="I30" s="157"/>
-      <c r="J30" s="158"/>
+      <c r="F30" s="127"/>
+      <c r="G30" s="128"/>
+      <c r="H30" s="128"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="129"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="32"/>
     </row>
     <row r="31" spans="1:13" ht="14" customHeight="1" thickBot="1">
-      <c r="A31" s="152" t="s">
+      <c r="A31" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="153"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="155"/>
+      <c r="B31" s="124"/>
+      <c r="C31" s="125"/>
+      <c r="D31" s="126"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="126"/>
-      <c r="G31" s="127"/>
-      <c r="H31" s="127"/>
-      <c r="I31" s="127"/>
-      <c r="J31" s="128"/>
+      <c r="F31" s="130"/>
+      <c r="G31" s="131"/>
+      <c r="H31" s="131"/>
+      <c r="I31" s="131"/>
+      <c r="J31" s="132"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="32"/>
@@ -24687,39 +24663,46 @@
       <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:10" ht="14" customHeight="1">
-      <c r="A33" s="121" t="s">
+      <c r="A33" s="155" t="s">
         <v>858</v>
       </c>
-      <c r="B33" s="121"/>
-      <c r="C33" s="121"/>
-      <c r="D33" s="121"/>
-      <c r="E33" s="121"/>
-      <c r="F33" s="121"/>
-      <c r="G33" s="121"/>
-      <c r="H33" s="121"/>
-      <c r="I33" s="121"/>
-      <c r="J33" s="121"/>
+      <c r="B33" s="155"/>
+      <c r="C33" s="155"/>
+      <c r="D33" s="155"/>
+      <c r="E33" s="155"/>
+      <c r="F33" s="155"/>
+      <c r="G33" s="155"/>
+      <c r="H33" s="155"/>
+      <c r="I33" s="155"/>
+      <c r="J33" s="155"/>
     </row>
     <row r="34" spans="1:10" ht="14" customHeight="1">
-      <c r="A34" s="121"/>
-      <c r="B34" s="121"/>
-      <c r="C34" s="121"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="121"/>
-      <c r="I34" s="121"/>
-      <c r="J34" s="121"/>
+      <c r="A34" s="155"/>
+      <c r="B34" s="155"/>
+      <c r="C34" s="155"/>
+      <c r="D34" s="155"/>
+      <c r="E34" s="155"/>
+      <c r="F34" s="155"/>
+      <c r="G34" s="155"/>
+      <c r="H34" s="155"/>
+      <c r="I34" s="155"/>
+      <c r="J34" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F29:J31"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="A33:J34"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A6:D6"/>
@@ -24733,19 +24716,12 @@
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F17:H17"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="A33:J34"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F29:J31"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F25:J26"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -24810,53 +24786,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="181" t="s">
         <v>845</v>
       </c>
-      <c r="B1" s="169"/>
+      <c r="B1" s="182"/>
       <c r="C1" s="114"/>
-      <c r="D1" s="179" t="s">
+      <c r="D1" s="171" t="s">
         <v>740</v>
       </c>
-      <c r="E1" s="180"/>
+      <c r="E1" s="172"/>
       <c r="F1" s="70"/>
-      <c r="G1" s="179" t="s">
+      <c r="G1" s="171" t="s">
         <v>741</v>
       </c>
-      <c r="H1" s="180"/>
+      <c r="H1" s="172"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A2" s="168"/>
-      <c r="B2" s="169"/>
+      <c r="A2" s="181"/>
+      <c r="B2" s="182"/>
       <c r="C2" s="114"/>
-      <c r="D2" s="181" t="s">
+      <c r="D2" s="173" t="s">
         <v>634</v>
       </c>
-      <c r="E2" s="182"/>
+      <c r="E2" s="174"/>
       <c r="F2" s="70"/>
-      <c r="G2" s="181" t="s">
+      <c r="G2" s="173" t="s">
         <v>634</v>
       </c>
-      <c r="H2" s="182"/>
+      <c r="H2" s="174"/>
       <c r="J2" s="72" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="23" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
-      <c r="B3" s="169"/>
+      <c r="A3" s="181"/>
+      <c r="B3" s="182"/>
       <c r="C3" s="115"/>
-      <c r="D3" s="183">
+      <c r="D3" s="175">
         <f>MAX(0,MIN(1,IF(($A$6+$D$6) &lt;= 0.95, ROUND($A$6+$D$6,2), FLOOR((0.95+($A$6+$D$6-0.95)/5),0.01))))</f>
         <v>0.78</v>
       </c>
-      <c r="E3" s="184"/>
+      <c r="E3" s="176"/>
       <c r="F3" s="71"/>
-      <c r="G3" s="183">
+      <c r="G3" s="175">
         <f>MAX(0,MIN(1,IF(($A$6+$G$6+J3) &lt;= 0.95, ROUND($A$6+$G$6+J3,2), FLOOR((0.95+($A$6+$G$6+J3-0.95)/5),0.01))))</f>
         <v>0.79</v>
       </c>
-      <c r="H3" s="184"/>
+      <c r="H3" s="176"/>
       <c r="J3" s="116">
         <f>IF(J6 &gt; 0.06, 0, 0.03-J6/2)</f>
         <v>2.375E-2</v>
@@ -24874,30 +24850,30 @@
       <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="14" customHeight="1" thickBot="1">
-      <c r="A5" s="170" t="s">
+      <c r="A5" s="183" t="s">
         <v>635</v>
       </c>
-      <c r="B5" s="171"/>
+      <c r="B5" s="184"/>
       <c r="C5" s="25"/>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="146" t="s">
         <v>735</v>
       </c>
-      <c r="E5" s="137"/>
+      <c r="E5" s="148"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="135" t="s">
+      <c r="G5" s="146" t="s">
         <v>735</v>
       </c>
-      <c r="H5" s="137"/>
+      <c r="H5" s="148"/>
       <c r="J5" s="72" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14" customHeight="1" thickBot="1">
-      <c r="A6" s="172">
+      <c r="A6" s="185">
         <f>'Game Data'!$J$22+Submission!$E$16</f>
         <v>0.77</v>
       </c>
-      <c r="B6" s="173"/>
+      <c r="B6" s="186"/>
       <c r="C6" s="103"/>
       <c r="D6" s="166">
         <f>E15+E24+E33+E42+E51+E60</f>
@@ -24919,15 +24895,15 @@
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
       <c r="C7" s="103"/>
-      <c r="D7" s="175" t="s">
+      <c r="D7" s="177" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="175"/>
+      <c r="E7" s="177"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="175" t="s">
+      <c r="G7" s="177" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="175"/>
+      <c r="H7" s="177"/>
       <c r="J7" s="74"/>
     </row>
     <row r="8" spans="1:10" ht="14" customHeight="1" thickBot="1">
@@ -24951,7 +24927,7 @@
       <c r="H8" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="176" t="s">
+      <c r="J8" s="178" t="s">
         <v>729</v>
       </c>
     </row>
@@ -24981,7 +24957,7 @@
         <f t="shared" ref="H9:H14" si="1">$B9*G9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="177"/>
+      <c r="J9" s="179"/>
     </row>
     <row r="10" spans="1:10" ht="14" customHeight="1" thickBot="1">
       <c r="A10" s="9" t="str">
@@ -25009,7 +24985,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="178"/>
+      <c r="J10" s="180"/>
     </row>
     <row r="11" spans="1:10" ht="14" customHeight="1" thickBot="1">
       <c r="A11" s="9" t="str">
@@ -25095,7 +25071,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="185" t="s">
+      <c r="J13" s="168" t="s">
         <v>731</v>
       </c>
     </row>
@@ -25125,7 +25101,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J14" s="185"/>
+      <c r="J14" s="168"/>
     </row>
     <row r="15" spans="1:10" ht="14" customHeight="1">
       <c r="A15" s="3"/>
@@ -25146,22 +25122,22 @@
         <f>SUM(H9:H14)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="185"/>
+      <c r="J15" s="168"/>
     </row>
     <row r="16" spans="1:10" ht="14" customHeight="1" thickBot="1">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
       <c r="C16" s="103"/>
-      <c r="D16" s="174" t="s">
+      <c r="D16" s="170" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="174"/>
+      <c r="E16" s="170"/>
       <c r="F16" s="103"/>
-      <c r="G16" s="174" t="s">
+      <c r="G16" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="174"/>
-      <c r="J16" s="185"/>
+      <c r="H16" s="170"/>
+      <c r="J16" s="168"/>
     </row>
     <row r="17" spans="1:10" ht="14" customHeight="1" thickBot="1">
       <c r="A17" s="1" t="s">
@@ -25184,7 +25160,7 @@
       <c r="H17" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="185"/>
+      <c r="J17" s="168"/>
     </row>
     <row r="18" spans="1:10" ht="14" customHeight="1" thickBot="1">
       <c r="A18" s="53" t="str">
@@ -25212,7 +25188,7 @@
         <f t="shared" ref="H18:H23" si="3">$B18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="186"/>
+      <c r="J18" s="169"/>
     </row>
     <row r="19" spans="1:10" ht="14" customHeight="1" thickBot="1">
       <c r="A19" s="9" t="str">
@@ -25388,15 +25364,15 @@
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
       <c r="C25" s="103"/>
-      <c r="D25" s="174" t="s">
+      <c r="D25" s="170" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="174"/>
+      <c r="E25" s="170"/>
       <c r="F25" s="103"/>
-      <c r="G25" s="174" t="s">
+      <c r="G25" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="H25" s="174"/>
+      <c r="H25" s="170"/>
       <c r="J25" s="78" t="s">
         <v>647</v>
       </c>
@@ -25615,15 +25591,15 @@
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
       <c r="C34" s="103"/>
-      <c r="D34" s="174" t="s">
+      <c r="D34" s="170" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="174"/>
+      <c r="E34" s="170"/>
       <c r="F34" s="103"/>
-      <c r="G34" s="174" t="s">
+      <c r="G34" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="H34" s="174"/>
+      <c r="H34" s="170"/>
     </row>
     <row r="35" spans="1:8" ht="14" customHeight="1" thickBot="1">
       <c r="A35" s="1" t="s">
@@ -25833,15 +25809,15 @@
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
       <c r="C43" s="103"/>
-      <c r="D43" s="174" t="s">
+      <c r="D43" s="170" t="s">
         <v>74</v>
       </c>
-      <c r="E43" s="174"/>
+      <c r="E43" s="170"/>
       <c r="F43" s="103"/>
-      <c r="G43" s="174" t="s">
+      <c r="G43" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="H43" s="174"/>
+      <c r="H43" s="170"/>
     </row>
     <row r="44" spans="1:8" ht="14" customHeight="1" thickBot="1">
       <c r="A44" s="1" t="s">
@@ -26051,15 +26027,15 @@
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
       <c r="C52" s="103"/>
-      <c r="D52" s="174" t="s">
+      <c r="D52" s="170" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="174"/>
+      <c r="E52" s="170"/>
       <c r="F52" s="103"/>
-      <c r="G52" s="174" t="s">
+      <c r="G52" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="H52" s="174"/>
+      <c r="H52" s="170"/>
     </row>
     <row r="53" spans="1:8" ht="14" customHeight="1" thickBot="1">
       <c r="A53" s="1" t="s">
@@ -26267,6 +26243,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="J13:J18"/>
@@ -26275,25 +26270,6 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -26325,14 +26301,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14" customHeight="1" thickBot="1">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="199" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="192"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="201"/>
     </row>
     <row r="2" spans="1:6" ht="43" customHeight="1" thickBot="1">
       <c r="A2" s="187" t="s">
@@ -26345,14 +26321,14 @@
       <c r="F2" s="189"/>
     </row>
     <row r="3" spans="1:6" ht="43" customHeight="1" thickBot="1">
-      <c r="A3" s="193" t="s">
+      <c r="A3" s="214" t="s">
         <v>880</v>
       </c>
-      <c r="B3" s="194"/>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="195"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="216"/>
     </row>
     <row r="4" spans="1:6" ht="29" customHeight="1" thickBot="1">
       <c r="A4" s="187" t="s">
@@ -26365,14 +26341,14 @@
       <c r="F4" s="189"/>
     </row>
     <row r="5" spans="1:6" ht="29" customHeight="1" thickBot="1">
-      <c r="A5" s="196" t="s">
+      <c r="A5" s="217" t="s">
         <v>879</v>
       </c>
-      <c r="B5" s="197"/>
-      <c r="C5" s="197"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="197"/>
-      <c r="F5" s="198"/>
+      <c r="B5" s="218"/>
+      <c r="C5" s="218"/>
+      <c r="D5" s="218"/>
+      <c r="E5" s="218"/>
+      <c r="F5" s="219"/>
     </row>
     <row r="6" spans="1:6" ht="14" customHeight="1" thickBot="1">
       <c r="A6" s="6"/>
@@ -26401,10 +26377,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="14" customHeight="1">
-      <c r="A8" s="193" t="s">
+      <c r="A8" s="214" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="194"/>
+      <c r="B8" s="215"/>
       <c r="C8" s="17">
         <v>0</v>
       </c>
@@ -26420,10 +26396,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="14" customHeight="1">
-      <c r="A9" s="200" t="s">
+      <c r="A9" s="221" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="201"/>
+      <c r="B9" s="222"/>
       <c r="C9" s="12">
         <v>0</v>
       </c>
@@ -26439,10 +26415,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="14" customHeight="1">
-      <c r="A10" s="202" t="s">
+      <c r="A10" s="223" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="202"/>
+      <c r="B10" s="223"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -26458,10 +26434,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="14" customHeight="1">
-      <c r="A11" s="202" t="s">
+      <c r="A11" s="223" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="223"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -26477,10 +26453,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="14" customHeight="1">
-      <c r="A12" s="202" t="s">
+      <c r="A12" s="223" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="202"/>
+      <c r="B12" s="223"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -26496,10 +26472,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="14" customHeight="1">
-      <c r="A13" s="200" t="s">
+      <c r="A13" s="221" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="201"/>
+      <c r="B13" s="222"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -26515,10 +26491,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14" customHeight="1">
-      <c r="A14" s="200" t="s">
+      <c r="A14" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="201"/>
+      <c r="B14" s="222"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -26534,10 +26510,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="14" customHeight="1" thickBot="1">
-      <c r="A15" s="203" t="s">
+      <c r="A15" s="224" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="204"/>
+      <c r="B15" s="225"/>
       <c r="C15" s="18">
         <v>0</v>
       </c>
@@ -26554,11 +26530,11 @@
     </row>
     <row r="16" spans="1:6" ht="14" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="199" t="s">
+      <c r="B16" s="220" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="199"/>
-      <c r="D16" s="199"/>
+      <c r="C16" s="220"/>
+      <c r="D16" s="220"/>
       <c r="E16" s="81">
         <f>SUM(E8:E15)</f>
         <v>0</v>
@@ -26577,13 +26553,13 @@
       <c r="A18" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="190" t="s">
+      <c r="B18" s="199" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="191"/>
-      <c r="D18" s="191"/>
-      <c r="E18" s="191"/>
-      <c r="F18" s="192"/>
+      <c r="C18" s="200"/>
+      <c r="D18" s="200"/>
+      <c r="E18" s="200"/>
+      <c r="F18" s="201"/>
     </row>
     <row r="19" spans="1:6" ht="29" customHeight="1" thickBot="1">
       <c r="A19" s="59" t="s">
@@ -26622,246 +26598,246 @@
       <c r="F21" s="189"/>
     </row>
     <row r="22" spans="1:6" ht="29" customHeight="1">
-      <c r="A22" s="205" t="s">
+      <c r="A22" s="202" t="s">
         <v>775</v>
       </c>
-      <c r="B22" s="208" t="s">
+      <c r="B22" s="205" t="s">
         <v>747</v>
       </c>
-      <c r="C22" s="209"/>
-      <c r="D22" s="209"/>
-      <c r="E22" s="209"/>
-      <c r="F22" s="210"/>
+      <c r="C22" s="206"/>
+      <c r="D22" s="206"/>
+      <c r="E22" s="206"/>
+      <c r="F22" s="207"/>
     </row>
     <row r="23" spans="1:6" ht="15.5">
-      <c r="A23" s="206"/>
-      <c r="B23" s="211"/>
-      <c r="C23" s="212"/>
-      <c r="D23" s="212"/>
-      <c r="E23" s="212"/>
-      <c r="F23" s="213"/>
+      <c r="A23" s="203"/>
+      <c r="B23" s="208"/>
+      <c r="C23" s="209"/>
+      <c r="D23" s="209"/>
+      <c r="E23" s="209"/>
+      <c r="F23" s="210"/>
     </row>
     <row r="24" spans="1:6" ht="15.5">
-      <c r="A24" s="206"/>
-      <c r="B24" s="214" t="s">
+      <c r="A24" s="203"/>
+      <c r="B24" s="211" t="s">
         <v>748</v>
       </c>
-      <c r="C24" s="215"/>
-      <c r="D24" s="215"/>
-      <c r="E24" s="215"/>
-      <c r="F24" s="216"/>
+      <c r="C24" s="212"/>
+      <c r="D24" s="212"/>
+      <c r="E24" s="212"/>
+      <c r="F24" s="213"/>
     </row>
     <row r="25" spans="1:6" ht="15.5">
-      <c r="A25" s="206"/>
-      <c r="B25" s="217" t="s">
+      <c r="A25" s="203"/>
+      <c r="B25" s="193" t="s">
         <v>749</v>
       </c>
-      <c r="C25" s="218"/>
-      <c r="D25" s="218"/>
-      <c r="E25" s="218"/>
-      <c r="F25" s="219"/>
+      <c r="C25" s="194"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="194"/>
+      <c r="F25" s="195"/>
     </row>
     <row r="26" spans="1:6" ht="15.5">
-      <c r="A26" s="206"/>
-      <c r="B26" s="211"/>
-      <c r="C26" s="212"/>
-      <c r="D26" s="212"/>
-      <c r="E26" s="212"/>
-      <c r="F26" s="213"/>
+      <c r="A26" s="203"/>
+      <c r="B26" s="208"/>
+      <c r="C26" s="209"/>
+      <c r="D26" s="209"/>
+      <c r="E26" s="209"/>
+      <c r="F26" s="210"/>
     </row>
     <row r="27" spans="1:6" ht="43" customHeight="1">
-      <c r="A27" s="206"/>
-      <c r="B27" s="217" t="s">
+      <c r="A27" s="203"/>
+      <c r="B27" s="193" t="s">
         <v>750</v>
       </c>
-      <c r="C27" s="218"/>
-      <c r="D27" s="218"/>
-      <c r="E27" s="218"/>
-      <c r="F27" s="219"/>
+      <c r="C27" s="194"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="194"/>
+      <c r="F27" s="195"/>
     </row>
     <row r="28" spans="1:6" ht="15.5">
-      <c r="A28" s="206"/>
-      <c r="B28" s="211"/>
-      <c r="C28" s="212"/>
-      <c r="D28" s="212"/>
-      <c r="E28" s="212"/>
-      <c r="F28" s="213"/>
+      <c r="A28" s="203"/>
+      <c r="B28" s="208"/>
+      <c r="C28" s="209"/>
+      <c r="D28" s="209"/>
+      <c r="E28" s="209"/>
+      <c r="F28" s="210"/>
     </row>
     <row r="29" spans="1:6" ht="15.5">
-      <c r="A29" s="206"/>
-      <c r="B29" s="217" t="s">
+      <c r="A29" s="203"/>
+      <c r="B29" s="193" t="s">
         <v>751</v>
       </c>
-      <c r="C29" s="218"/>
-      <c r="D29" s="218"/>
-      <c r="E29" s="218"/>
-      <c r="F29" s="219"/>
+      <c r="C29" s="194"/>
+      <c r="D29" s="194"/>
+      <c r="E29" s="194"/>
+      <c r="F29" s="195"/>
     </row>
     <row r="30" spans="1:6" ht="15.5">
-      <c r="A30" s="206"/>
-      <c r="B30" s="217" t="s">
+      <c r="A30" s="203"/>
+      <c r="B30" s="193" t="s">
         <v>752</v>
       </c>
-      <c r="C30" s="218"/>
-      <c r="D30" s="218"/>
-      <c r="E30" s="218"/>
-      <c r="F30" s="219"/>
+      <c r="C30" s="194"/>
+      <c r="D30" s="194"/>
+      <c r="E30" s="194"/>
+      <c r="F30" s="195"/>
     </row>
     <row r="31" spans="1:6" ht="15.5">
-      <c r="A31" s="206"/>
-      <c r="B31" s="217" t="s">
+      <c r="A31" s="203"/>
+      <c r="B31" s="193" t="s">
         <v>753</v>
       </c>
-      <c r="C31" s="218"/>
-      <c r="D31" s="218"/>
-      <c r="E31" s="218"/>
-      <c r="F31" s="219"/>
+      <c r="C31" s="194"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="194"/>
+      <c r="F31" s="195"/>
     </row>
     <row r="32" spans="1:6" ht="15.5">
-      <c r="A32" s="206"/>
-      <c r="B32" s="217" t="s">
+      <c r="A32" s="203"/>
+      <c r="B32" s="193" t="s">
         <v>754</v>
       </c>
-      <c r="C32" s="218"/>
-      <c r="D32" s="218"/>
-      <c r="E32" s="218"/>
-      <c r="F32" s="219"/>
+      <c r="C32" s="194"/>
+      <c r="D32" s="194"/>
+      <c r="E32" s="194"/>
+      <c r="F32" s="195"/>
     </row>
     <row r="33" spans="1:6" ht="15.5">
-      <c r="A33" s="206"/>
-      <c r="B33" s="217" t="s">
+      <c r="A33" s="203"/>
+      <c r="B33" s="193" t="s">
         <v>755</v>
       </c>
-      <c r="C33" s="218"/>
-      <c r="D33" s="218"/>
-      <c r="E33" s="218"/>
-      <c r="F33" s="219"/>
+      <c r="C33" s="194"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="194"/>
+      <c r="F33" s="195"/>
     </row>
     <row r="34" spans="1:6" ht="15.5">
-      <c r="A34" s="206"/>
-      <c r="B34" s="217" t="s">
+      <c r="A34" s="203"/>
+      <c r="B34" s="193" t="s">
         <v>756</v>
       </c>
-      <c r="C34" s="218"/>
-      <c r="D34" s="218"/>
-      <c r="E34" s="218"/>
-      <c r="F34" s="219"/>
+      <c r="C34" s="194"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="194"/>
+      <c r="F34" s="195"/>
     </row>
     <row r="35" spans="1:6" ht="15.5">
-      <c r="A35" s="206"/>
-      <c r="B35" s="217" t="s">
+      <c r="A35" s="203"/>
+      <c r="B35" s="193" t="s">
         <v>757</v>
       </c>
-      <c r="C35" s="218"/>
-      <c r="D35" s="218"/>
-      <c r="E35" s="218"/>
-      <c r="F35" s="219"/>
+      <c r="C35" s="194"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="194"/>
+      <c r="F35" s="195"/>
     </row>
     <row r="36" spans="1:6" ht="16" thickBot="1">
-      <c r="A36" s="207"/>
-      <c r="B36" s="220" t="s">
+      <c r="A36" s="204"/>
+      <c r="B36" s="196" t="s">
         <v>758</v>
       </c>
-      <c r="C36" s="221"/>
-      <c r="D36" s="221"/>
-      <c r="E36" s="221"/>
-      <c r="F36" s="222"/>
+      <c r="C36" s="197"/>
+      <c r="D36" s="197"/>
+      <c r="E36" s="197"/>
+      <c r="F36" s="198"/>
     </row>
     <row r="37" spans="1:6" ht="58" customHeight="1" thickBot="1">
       <c r="A37" s="54" t="s">
         <v>774</v>
       </c>
-      <c r="B37" s="223" t="s">
+      <c r="B37" s="190" t="s">
         <v>759</v>
       </c>
-      <c r="C37" s="224"/>
-      <c r="D37" s="224"/>
-      <c r="E37" s="224"/>
-      <c r="F37" s="225"/>
+      <c r="C37" s="191"/>
+      <c r="D37" s="191"/>
+      <c r="E37" s="191"/>
+      <c r="F37" s="192"/>
     </row>
     <row r="38" spans="1:6" ht="58" customHeight="1" thickBot="1">
       <c r="A38" s="54" t="s">
         <v>773</v>
       </c>
-      <c r="B38" s="223" t="s">
+      <c r="B38" s="190" t="s">
         <v>760</v>
       </c>
-      <c r="C38" s="224"/>
-      <c r="D38" s="224"/>
-      <c r="E38" s="224"/>
-      <c r="F38" s="225"/>
+      <c r="C38" s="191"/>
+      <c r="D38" s="191"/>
+      <c r="E38" s="191"/>
+      <c r="F38" s="192"/>
     </row>
     <row r="39" spans="1:6" ht="16" thickBot="1">
       <c r="A39" s="54" t="s">
         <v>772</v>
       </c>
-      <c r="B39" s="223" t="s">
+      <c r="B39" s="190" t="s">
         <v>761</v>
       </c>
-      <c r="C39" s="224"/>
-      <c r="D39" s="224"/>
-      <c r="E39" s="224"/>
-      <c r="F39" s="225"/>
+      <c r="C39" s="191"/>
+      <c r="D39" s="191"/>
+      <c r="E39" s="191"/>
+      <c r="F39" s="192"/>
     </row>
     <row r="40" spans="1:6" ht="39.5" thickBot="1">
       <c r="A40" s="55" t="s">
         <v>766</v>
       </c>
-      <c r="B40" s="223" t="s">
+      <c r="B40" s="190" t="s">
         <v>762</v>
       </c>
-      <c r="C40" s="224"/>
-      <c r="D40" s="224"/>
-      <c r="E40" s="224"/>
-      <c r="F40" s="225"/>
+      <c r="C40" s="191"/>
+      <c r="D40" s="191"/>
+      <c r="E40" s="191"/>
+      <c r="F40" s="192"/>
     </row>
     <row r="41" spans="1:6" ht="29" customHeight="1" thickBot="1">
       <c r="A41" s="54" t="s">
         <v>771</v>
       </c>
-      <c r="B41" s="223" t="s">
+      <c r="B41" s="190" t="s">
         <v>763</v>
       </c>
-      <c r="C41" s="224"/>
-      <c r="D41" s="224"/>
-      <c r="E41" s="224"/>
-      <c r="F41" s="225"/>
+      <c r="C41" s="191"/>
+      <c r="D41" s="191"/>
+      <c r="E41" s="191"/>
+      <c r="F41" s="192"/>
     </row>
     <row r="42" spans="1:6" ht="16" thickBot="1">
       <c r="A42" s="54" t="s">
         <v>770</v>
       </c>
-      <c r="B42" s="223" t="s">
+      <c r="B42" s="190" t="s">
         <v>764</v>
       </c>
-      <c r="C42" s="224"/>
-      <c r="D42" s="224"/>
-      <c r="E42" s="224"/>
-      <c r="F42" s="225"/>
+      <c r="C42" s="191"/>
+      <c r="D42" s="191"/>
+      <c r="E42" s="191"/>
+      <c r="F42" s="192"/>
     </row>
     <row r="43" spans="1:6" ht="39.5" thickBot="1">
       <c r="A43" s="55" t="s">
         <v>767</v>
       </c>
-      <c r="B43" s="223" t="s">
+      <c r="B43" s="190" t="s">
         <v>768</v>
       </c>
-      <c r="C43" s="224"/>
-      <c r="D43" s="224"/>
-      <c r="E43" s="224"/>
-      <c r="F43" s="225"/>
+      <c r="C43" s="191"/>
+      <c r="D43" s="191"/>
+      <c r="E43" s="191"/>
+      <c r="F43" s="192"/>
     </row>
     <row r="44" spans="1:6" ht="29" customHeight="1" thickBot="1">
       <c r="A44" s="54" t="s">
         <v>769</v>
       </c>
-      <c r="B44" s="223" t="s">
+      <c r="B44" s="190" t="s">
         <v>765</v>
       </c>
-      <c r="C44" s="224"/>
-      <c r="D44" s="224"/>
-      <c r="E44" s="224"/>
-      <c r="F44" s="225"/>
+      <c r="C44" s="191"/>
+      <c r="D44" s="191"/>
+      <c r="E44" s="191"/>
+      <c r="F44" s="192"/>
     </row>
     <row r="45" spans="1:6" ht="28" customHeight="1" thickBot="1">
       <c r="A45" s="54" t="s">
@@ -26877,17 +26853,22 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="A22:A36"/>
@@ -26904,22 +26885,17 @@
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -26935,8 +26911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="C92" zoomScale="145" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="14" customHeight="1"/>
@@ -28006,7 +27982,7 @@
         <v>125</v>
       </c>
       <c r="D54" s="55" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>68</v>
@@ -28705,9 +28681,7 @@
       <c r="C90" s="55" t="s">
         <v>178</v>
       </c>
-      <c r="D90" s="55" t="s">
-        <v>893</v>
-      </c>
+      <c r="D90" s="55"/>
       <c r="E90" s="8" t="s">
         <v>68</v>
       </c>
@@ -28745,9 +28719,7 @@
       <c r="C92" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="D92" s="120" t="s">
-        <v>894</v>
-      </c>
+      <c r="D92" s="120"/>
       <c r="E92" s="8" t="s">
         <v>68</v>
       </c>
@@ -28786,7 +28758,7 @@
         <v>655</v>
       </c>
       <c r="D94" s="120" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>68</v>
@@ -28885,7 +28857,7 @@
         <v>849</v>
       </c>
       <c r="D99" s="120" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>68</v>
@@ -29197,7 +29169,7 @@
         <v>832</v>
       </c>
       <c r="D115" s="120" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>66</v>
@@ -29401,6 +29373,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="C2:D9"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A39:B39"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A117:B117"/>
     <mergeCell ref="A50:B50"/>
@@ -29410,13 +29389,6 @@
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="A112:B112"/>
     <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="C2:D9"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <conditionalFormatting sqref="A97 A11:A18 A89:A91 A82:A86 A94:A95 A117:A250 A103:A105 A107:A111 A58:A68 A50:A56 A40:A42 A33:A38 A20:A29">
     <cfRule type="beginsWith" dxfId="1344" priority="941" stopIfTrue="1" operator="beginsWith" text="Exceptional">
@@ -32348,7 +32320,7 @@
       </c>
       <c r="G62" s="55"/>
     </row>
-    <row r="63" spans="1:7" ht="39.5" thickBot="1">
+    <row r="63" spans="1:7" ht="26.5" thickBot="1">
       <c r="A63" s="118" t="s">
         <v>81</v>
       </c>
@@ -34352,7 +34324,7 @@
       </c>
       <c r="G36" s="55"/>
     </row>
-    <row r="37" spans="1:7" s="24" customFormat="1" ht="65.5" thickBot="1">
+    <row r="37" spans="1:7" s="24" customFormat="1" ht="52.5" thickBot="1">
       <c r="A37" s="63" t="s">
         <v>79</v>
       </c>
@@ -34390,7 +34362,7 @@
       </c>
       <c r="G38" s="55"/>
     </row>
-    <row r="39" spans="1:7" s="24" customFormat="1" ht="26.5" thickBot="1">
+    <row r="39" spans="1:7" s="24" customFormat="1" ht="16" thickBot="1">
       <c r="A39" s="64" t="s">
         <v>81</v>
       </c>
@@ -37934,7 +37906,7 @@
       </c>
       <c r="G54" s="55"/>
     </row>
-    <row r="55" spans="1:7" s="24" customFormat="1" ht="39.5" thickBot="1">
+    <row r="55" spans="1:7" s="24" customFormat="1" ht="26.5" thickBot="1">
       <c r="A55" s="89" t="s">
         <v>81</v>
       </c>

</xml_diff>